<commit_message>
new selection files + MC test
</commit_message>
<xml_diff>
--- a/Aluminium new data/compositions_al.xlsx
+++ b/Aluminium new data/compositions_al.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Desktop\libs\Aluminium new data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD990A07-4A73-4DE9-AACC-B0541DA60525}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697B1D4F-5FF4-43EB-9085-38C2CE405175}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -293,7 +293,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -384,6 +384,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -408,7 +414,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -522,6 +528,17 @@
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="4" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="16" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="16" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -880,8 +897,8 @@
   </sheetPr>
   <dimension ref="A2:AY49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -1253,87 +1270,87 @@
         <v>91.414000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="13">
+    <row r="9" spans="1:51" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="51">
         <v>4</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="16">
+      <c r="C9" s="53"/>
+      <c r="D9" s="54">
         <v>9.3620000000000001</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="54">
         <v>0.86499999999999999</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="53">
         <v>6.3700000000000007E-2</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="53">
         <f>AVERAGE(0.0877,0.0859)</f>
         <v>8.6800000000000002E-2</v>
       </c>
-      <c r="H9" s="28">
+      <c r="H9" s="53">
         <v>0.41349999999999998</v>
       </c>
-      <c r="I9" s="22">
+      <c r="I9" s="54">
         <v>1.0109999999999999</v>
       </c>
-      <c r="J9" s="23">
+      <c r="J9" s="54">
         <v>3.4780000000000002</v>
       </c>
-      <c r="K9" s="28">
+      <c r="K9" s="53">
         <v>0.38569999999999999</v>
       </c>
-      <c r="L9" s="28">
+      <c r="L9" s="53">
         <v>0.1075</v>
       </c>
-      <c r="M9" s="28">
+      <c r="M9" s="53">
         <v>9.1000000000000004E-3</v>
       </c>
-      <c r="N9" s="28">
+      <c r="N9" s="53">
         <v>5.7200000000000001E-2</v>
       </c>
-      <c r="O9" s="12">
+      <c r="O9" s="55">
         <v>84.160499999999999</v>
       </c>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="5"/>
-      <c r="Y9" s="5"/>
-      <c r="Z9" s="5"/>
-      <c r="AA9" s="5"/>
-      <c r="AB9" s="5"/>
-      <c r="AC9" s="5"/>
-      <c r="AD9" s="5"/>
-      <c r="AE9" s="5"/>
-      <c r="AF9" s="5"/>
-      <c r="AG9" s="5"/>
-      <c r="AH9" s="5"/>
-      <c r="AI9" s="5"/>
-      <c r="AJ9" s="5"/>
-      <c r="AK9" s="5"/>
-      <c r="AL9" s="5"/>
-      <c r="AM9" s="5"/>
-      <c r="AN9" s="5"/>
-      <c r="AO9" s="5"/>
-      <c r="AP9" s="5"/>
-      <c r="AQ9" s="5"/>
-      <c r="AR9" s="5"/>
-      <c r="AS9" s="5"/>
-      <c r="AT9" s="8"/>
-      <c r="AU9" s="8"/>
-      <c r="AV9" s="8"/>
-      <c r="AW9" s="8"/>
-      <c r="AX9" s="8"/>
-      <c r="AY9" s="8"/>
+      <c r="P9" s="56"/>
+      <c r="Q9" s="56"/>
+      <c r="R9" s="56"/>
+      <c r="S9" s="56"/>
+      <c r="T9" s="56"/>
+      <c r="U9" s="56"/>
+      <c r="V9" s="56"/>
+      <c r="W9" s="56"/>
+      <c r="X9" s="56"/>
+      <c r="Y9" s="56"/>
+      <c r="Z9" s="56"/>
+      <c r="AA9" s="56"/>
+      <c r="AB9" s="56"/>
+      <c r="AC9" s="56"/>
+      <c r="AD9" s="56"/>
+      <c r="AE9" s="56"/>
+      <c r="AF9" s="56"/>
+      <c r="AG9" s="56"/>
+      <c r="AH9" s="56"/>
+      <c r="AI9" s="56"/>
+      <c r="AJ9" s="56"/>
+      <c r="AK9" s="56"/>
+      <c r="AL9" s="56"/>
+      <c r="AM9" s="56"/>
+      <c r="AN9" s="56"/>
+      <c r="AO9" s="56"/>
+      <c r="AP9" s="56"/>
+      <c r="AQ9" s="56"/>
+      <c r="AR9" s="56"/>
+      <c r="AS9" s="56"/>
+      <c r="AT9" s="56"/>
+      <c r="AU9" s="56"/>
+      <c r="AV9" s="56"/>
+      <c r="AW9" s="56"/>
+      <c r="AX9" s="56"/>
+      <c r="AY9" s="56"/>
     </row>
     <row r="10" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A10" s="44">
@@ -2008,87 +2025,87 @@
         <v>93.257400000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="13">
+    <row r="21" spans="1:51" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="51">
         <v>16</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="16">
+      <c r="C21" s="53"/>
+      <c r="D21" s="54">
         <v>9.3620000000000001</v>
       </c>
-      <c r="E21" s="25">
+      <c r="E21" s="54">
         <v>0.86499999999999999</v>
       </c>
-      <c r="F21" s="28">
+      <c r="F21" s="53">
         <v>6.3700000000000007E-2</v>
       </c>
-      <c r="G21" s="28">
+      <c r="G21" s="53">
         <f>AVERAGE(0.0877,0.0859)</f>
         <v>8.6800000000000002E-2</v>
       </c>
-      <c r="H21" s="28">
+      <c r="H21" s="53">
         <v>0.41349999999999998</v>
       </c>
-      <c r="I21" s="22">
+      <c r="I21" s="54">
         <v>1.0109999999999999</v>
       </c>
-      <c r="J21" s="23">
+      <c r="J21" s="54">
         <v>3.4780000000000002</v>
       </c>
-      <c r="K21" s="28">
+      <c r="K21" s="53">
         <v>0.38569999999999999</v>
       </c>
-      <c r="L21" s="28">
+      <c r="L21" s="53">
         <v>0.1075</v>
       </c>
-      <c r="M21" s="28">
+      <c r="M21" s="53">
         <v>9.1000000000000004E-3</v>
       </c>
-      <c r="N21" s="28">
+      <c r="N21" s="53">
         <v>5.7200000000000001E-2</v>
       </c>
-      <c r="O21" s="12">
+      <c r="O21" s="55">
         <v>84.160499999999999</v>
       </c>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
-      <c r="U21" s="5"/>
-      <c r="V21" s="5"/>
-      <c r="W21" s="5"/>
-      <c r="X21" s="5"/>
-      <c r="Y21" s="5"/>
-      <c r="Z21" s="5"/>
-      <c r="AA21" s="5"/>
-      <c r="AB21" s="5"/>
-      <c r="AC21" s="5"/>
-      <c r="AD21" s="5"/>
-      <c r="AE21" s="5"/>
-      <c r="AF21" s="5"/>
-      <c r="AG21" s="5"/>
-      <c r="AH21" s="5"/>
-      <c r="AI21" s="5"/>
-      <c r="AJ21" s="5"/>
-      <c r="AK21" s="5"/>
-      <c r="AL21" s="5"/>
-      <c r="AM21" s="5"/>
-      <c r="AN21" s="5"/>
-      <c r="AO21" s="5"/>
-      <c r="AP21" s="5"/>
-      <c r="AQ21" s="5"/>
-      <c r="AR21" s="5"/>
-      <c r="AS21" s="5"/>
-      <c r="AT21" s="8"/>
-      <c r="AU21" s="8"/>
-      <c r="AV21" s="8"/>
-      <c r="AW21" s="8"/>
-      <c r="AX21" s="8"/>
-      <c r="AY21" s="8"/>
+      <c r="P21" s="56"/>
+      <c r="Q21" s="56"/>
+      <c r="R21" s="56"/>
+      <c r="S21" s="56"/>
+      <c r="T21" s="56"/>
+      <c r="U21" s="56"/>
+      <c r="V21" s="56"/>
+      <c r="W21" s="56"/>
+      <c r="X21" s="56"/>
+      <c r="Y21" s="56"/>
+      <c r="Z21" s="56"/>
+      <c r="AA21" s="56"/>
+      <c r="AB21" s="56"/>
+      <c r="AC21" s="56"/>
+      <c r="AD21" s="56"/>
+      <c r="AE21" s="56"/>
+      <c r="AF21" s="56"/>
+      <c r="AG21" s="56"/>
+      <c r="AH21" s="56"/>
+      <c r="AI21" s="56"/>
+      <c r="AJ21" s="56"/>
+      <c r="AK21" s="56"/>
+      <c r="AL21" s="56"/>
+      <c r="AM21" s="56"/>
+      <c r="AN21" s="56"/>
+      <c r="AO21" s="56"/>
+      <c r="AP21" s="56"/>
+      <c r="AQ21" s="56"/>
+      <c r="AR21" s="56"/>
+      <c r="AS21" s="56"/>
+      <c r="AT21" s="56"/>
+      <c r="AU21" s="56"/>
+      <c r="AV21" s="56"/>
+      <c r="AW21" s="56"/>
+      <c r="AX21" s="56"/>
+      <c r="AY21" s="56"/>
     </row>
     <row r="22" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A22" s="13">
@@ -2462,51 +2479,51 @@
       <c r="AY26" s="8"/>
     </row>
     <row r="27" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="13">
+      <c r="A27" s="51">
         <v>22</v>
       </c>
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="28"/>
-      <c r="D27" s="16">
+      <c r="C27" s="53"/>
+      <c r="D27" s="54">
         <v>9.3620000000000001</v>
       </c>
-      <c r="E27" s="25">
+      <c r="E27" s="54">
         <v>0.86499999999999999</v>
       </c>
-      <c r="F27" s="28">
+      <c r="F27" s="53">
         <v>6.3700000000000007E-2</v>
       </c>
-      <c r="G27" s="28">
+      <c r="G27" s="53">
         <f>AVERAGE(0.0877,0.0859)</f>
         <v>8.6800000000000002E-2</v>
       </c>
-      <c r="H27" s="28">
+      <c r="H27" s="53">
         <v>0.41349999999999998</v>
       </c>
-      <c r="I27" s="22">
+      <c r="I27" s="54">
         <v>1.0109999999999999</v>
       </c>
-      <c r="J27" s="23">
+      <c r="J27" s="54">
         <v>3.4780000000000002</v>
       </c>
-      <c r="K27" s="28">
+      <c r="K27" s="53">
         <v>0.38569999999999999</v>
       </c>
-      <c r="L27" s="28">
+      <c r="L27" s="53">
         <v>0.1075</v>
       </c>
-      <c r="M27" s="28">
+      <c r="M27" s="53">
         <v>9.1000000000000004E-3</v>
       </c>
-      <c r="N27" s="28">
+      <c r="N27" s="53">
         <v>5.7200000000000001E-2</v>
       </c>
-      <c r="O27" s="12">
+      <c r="O27" s="55">
         <v>84.160499999999999</v>
       </c>
-      <c r="P27" s="5"/>
+      <c r="P27" s="56"/>
       <c r="Q27" s="5"/>
       <c r="R27" s="5"/>
       <c r="S27" s="5"/>
@@ -2832,7 +2849,7 @@
         <v>96.721000000000004</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A33" s="13">
         <v>28</v>
       </c>
@@ -2853,7 +2870,7 @@
       <c r="N33" s="28"/>
       <c r="O33" s="29"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A34" s="13">
         <v>29</v>
       </c>
@@ -2900,53 +2917,89 @@
         <v>89.843000000000004</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A35" s="13">
+    <row r="35" spans="1:51" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="51">
         <v>30</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="28"/>
-      <c r="D35" s="16">
+      <c r="C35" s="53"/>
+      <c r="D35" s="54">
         <v>9.3620000000000001</v>
       </c>
-      <c r="E35" s="25">
+      <c r="E35" s="54">
         <v>0.86499999999999999</v>
       </c>
-      <c r="F35" s="28">
+      <c r="F35" s="53">
         <v>6.3700000000000007E-2</v>
       </c>
-      <c r="G35" s="28">
+      <c r="G35" s="53">
         <f>AVERAGE(0.0877,0.0859)</f>
         <v>8.6800000000000002E-2</v>
       </c>
-      <c r="H35" s="28">
+      <c r="H35" s="53">
         <v>0.41349999999999998</v>
       </c>
-      <c r="I35" s="22">
+      <c r="I35" s="54">
         <v>1.0109999999999999</v>
       </c>
-      <c r="J35" s="23">
+      <c r="J35" s="54">
         <v>3.4780000000000002</v>
       </c>
-      <c r="K35" s="28">
+      <c r="K35" s="53">
         <v>0.38569999999999999</v>
       </c>
-      <c r="L35" s="28">
+      <c r="L35" s="53">
         <v>0.1075</v>
       </c>
-      <c r="M35" s="28">
+      <c r="M35" s="53">
         <v>9.1000000000000004E-3</v>
       </c>
-      <c r="N35" s="28">
+      <c r="N35" s="53">
         <v>5.7200000000000001E-2</v>
       </c>
-      <c r="O35" s="12">
+      <c r="O35" s="55">
         <v>84.160499999999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P35" s="56"/>
+      <c r="Q35" s="56"/>
+      <c r="R35" s="56"/>
+      <c r="S35" s="56"/>
+      <c r="T35" s="56"/>
+      <c r="U35" s="56"/>
+      <c r="V35" s="56"/>
+      <c r="W35" s="56"/>
+      <c r="X35" s="56"/>
+      <c r="Y35" s="56"/>
+      <c r="Z35" s="56"/>
+      <c r="AA35" s="56"/>
+      <c r="AB35" s="56"/>
+      <c r="AC35" s="56"/>
+      <c r="AD35" s="56"/>
+      <c r="AE35" s="56"/>
+      <c r="AF35" s="56"/>
+      <c r="AG35" s="56"/>
+      <c r="AH35" s="56"/>
+      <c r="AI35" s="56"/>
+      <c r="AJ35" s="56"/>
+      <c r="AK35" s="56"/>
+      <c r="AL35" s="56"/>
+      <c r="AM35" s="56"/>
+      <c r="AN35" s="56"/>
+      <c r="AO35" s="56"/>
+      <c r="AP35" s="56"/>
+      <c r="AQ35" s="56"/>
+      <c r="AR35" s="56"/>
+      <c r="AS35" s="56"/>
+      <c r="AT35" s="56"/>
+      <c r="AU35" s="56"/>
+      <c r="AV35" s="56"/>
+      <c r="AW35" s="56"/>
+      <c r="AX35" s="56"/>
+      <c r="AY35" s="56"/>
+    </row>
+    <row r="36" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A36" s="13">
         <v>31</v>
       </c>
@@ -2993,7 +3046,7 @@
         <v>86.817999999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A37" s="13">
         <v>32</v>
       </c>
@@ -3040,7 +3093,7 @@
         <v>90.021000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A38" s="13">
         <v>33</v>
       </c>
@@ -3087,7 +3140,7 @@
         <v>97.15</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A39" s="13">
         <v>34</v>
       </c>
@@ -3134,7 +3187,7 @@
         <v>84.807000000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A40" s="13">
         <v>35</v>
       </c>
@@ -3179,7 +3232,7 @@
         <v>86.564999999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A41" s="13">
         <v>36</v>
       </c>
@@ -3224,7 +3277,7 @@
         <v>95.915400000000005</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A42" s="13">
         <v>37</v>
       </c>
@@ -3271,7 +3324,7 @@
         <v>84.777000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A43" s="13">
         <v>38</v>
       </c>
@@ -3316,7 +3369,7 @@
         <v>88.21</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A44" s="13">
         <v>39</v>
       </c>
@@ -3363,53 +3416,89 @@
         <v>90.453800000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A45" s="13">
+    <row r="45" spans="1:51" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="51">
         <v>40</v>
       </c>
-      <c r="B45" s="27" t="s">
+      <c r="B45" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="28"/>
-      <c r="D45" s="16">
+      <c r="C45" s="53"/>
+      <c r="D45" s="54">
         <v>9.3620000000000001</v>
       </c>
-      <c r="E45" s="25">
+      <c r="E45" s="54">
         <v>0.86499999999999999</v>
       </c>
-      <c r="F45" s="28">
+      <c r="F45" s="53">
         <v>6.3700000000000007E-2</v>
       </c>
-      <c r="G45" s="28">
+      <c r="G45" s="53">
         <f>AVERAGE(0.0877,0.0859)</f>
         <v>8.6800000000000002E-2</v>
       </c>
-      <c r="H45" s="28">
+      <c r="H45" s="53">
         <v>0.41349999999999998</v>
       </c>
-      <c r="I45" s="22">
+      <c r="I45" s="54">
         <v>1.0109999999999999</v>
       </c>
-      <c r="J45" s="23">
+      <c r="J45" s="54">
         <v>3.4780000000000002</v>
       </c>
-      <c r="K45" s="28">
+      <c r="K45" s="53">
         <v>0.38569999999999999</v>
       </c>
-      <c r="L45" s="28">
+      <c r="L45" s="53">
         <v>0.1075</v>
       </c>
-      <c r="M45" s="28">
+      <c r="M45" s="53">
         <v>9.1000000000000004E-3</v>
       </c>
-      <c r="N45" s="28">
+      <c r="N45" s="53">
         <v>5.7200000000000001E-2</v>
       </c>
-      <c r="O45" s="12">
+      <c r="O45" s="55">
         <v>84.160499999999999</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P45" s="56"/>
+      <c r="Q45" s="56"/>
+      <c r="R45" s="56"/>
+      <c r="S45" s="56"/>
+      <c r="T45" s="56"/>
+      <c r="U45" s="56"/>
+      <c r="V45" s="56"/>
+      <c r="W45" s="56"/>
+      <c r="X45" s="56"/>
+      <c r="Y45" s="56"/>
+      <c r="Z45" s="56"/>
+      <c r="AA45" s="56"/>
+      <c r="AB45" s="56"/>
+      <c r="AC45" s="56"/>
+      <c r="AD45" s="56"/>
+      <c r="AE45" s="56"/>
+      <c r="AF45" s="56"/>
+      <c r="AG45" s="56"/>
+      <c r="AH45" s="56"/>
+      <c r="AI45" s="56"/>
+      <c r="AJ45" s="56"/>
+      <c r="AK45" s="56"/>
+      <c r="AL45" s="56"/>
+      <c r="AM45" s="56"/>
+      <c r="AN45" s="56"/>
+      <c r="AO45" s="56"/>
+      <c r="AP45" s="56"/>
+      <c r="AQ45" s="56"/>
+      <c r="AR45" s="56"/>
+      <c r="AS45" s="56"/>
+      <c r="AT45" s="56"/>
+      <c r="AU45" s="56"/>
+      <c r="AV45" s="56"/>
+      <c r="AW45" s="56"/>
+      <c r="AX45" s="56"/>
+      <c r="AY45" s="56"/>
+    </row>
+    <row r="46" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A46" s="40" t="s">
         <v>57</v>
       </c>
@@ -3456,7 +3545,7 @@
         <v>99.999200000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A47" s="40" t="s">
         <v>57</v>
       </c>
@@ -3503,7 +3592,7 @@
         <v>84.790500000000009</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A48" s="40" t="s">
         <v>57</v>
       </c>

</xml_diff>